<commit_message>
updated Appendix2_RawData.xlsx, added Appendix2_RawData.pdf
</commit_message>
<xml_diff>
--- a/ExperimentData/Appendix2_ExperimentData/RawData.xlsx
+++ b/ExperimentData/Appendix2_ExperimentData/RawData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="18720" windowHeight="12150"/>
+    <workbookView windowWidth="19650" windowHeight="11610"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57">
   <si>
     <t>Table Appendix 2</t>
   </si>
@@ -35,6 +35,21 @@
   </si>
   <si>
     <t>t5</t>
+  </si>
+  <si>
+    <t>t6</t>
+  </si>
+  <si>
+    <t>t7</t>
+  </si>
+  <si>
+    <t>t8</t>
+  </si>
+  <si>
+    <t>t9</t>
+  </si>
+  <si>
+    <t>t10</t>
   </si>
   <si>
     <t>Row1_LCC</t>
@@ -182,7 +197,7 @@
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -204,16 +219,37 @@
       <charset val="134"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FFFF0000"/>
+      <name val="Times New Roman"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -257,6 +293,46 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="宋体"/>
@@ -278,65 +354,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -357,6 +378,36 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -370,6 +421,54 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -429,42 +528,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -472,48 +535,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -551,17 +572,26 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -581,15 +611,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -601,30 +622,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -648,6 +645,30 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -656,10 +677,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="23" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -668,137 +689,137 @@
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="14" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="18" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="26" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -813,6 +834,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1129,13 +1153,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:H128"/>
+  <dimension ref="A1:M128"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" topLeftCell="A105" workbookViewId="0">
-      <selection activeCell="H128" sqref="H128"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="A105" workbookViewId="0">
+      <selection activeCell="C105" sqref="C105"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="12.4" style="1" customWidth="1"/>
     <col min="2" max="2" width="10.6666666666667" style="1" customWidth="1"/>
@@ -1147,7 +1171,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="3:8">
+    <row r="2" spans="3:13">
       <c r="C2" s="2" t="s">
         <v>1</v>
       </c>
@@ -1163,16 +1187,31 @@
       <c r="G2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:8">
+      <c r="I2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
       <c r="A3" s="1" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D3" s="1">
         <v>1.22</v>
@@ -1189,10 +1228,25 @@
       <c r="H3" s="1">
         <v>1.22</v>
       </c>
-    </row>
-    <row r="4" spans="2:8">
+      <c r="I3" s="1">
+        <v>1.23</v>
+      </c>
+      <c r="J3" s="1">
+        <v>1.22</v>
+      </c>
+      <c r="K3" s="1">
+        <v>1.23</v>
+      </c>
+      <c r="L3" s="1">
+        <v>1.23</v>
+      </c>
+      <c r="M3" s="1">
+        <v>1.22</v>
+      </c>
+    </row>
+    <row r="4" spans="2:13">
       <c r="B4" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D4" s="1">
         <v>0.03</v>
@@ -1209,10 +1263,25 @@
       <c r="H4" s="1">
         <v>0.08</v>
       </c>
-    </row>
-    <row r="5" spans="2:8">
+      <c r="I4" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="J4" s="1">
+        <v>0.04</v>
+      </c>
+      <c r="K4" s="1">
+        <v>0.08</v>
+      </c>
+      <c r="L4" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="M4" s="1">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="5" spans="2:13">
       <c r="B5" s="1" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D5" s="1">
         <v>1.19</v>
@@ -1229,13 +1298,28 @@
       <c r="H5" s="1">
         <v>1.14</v>
       </c>
-    </row>
-    <row r="6" spans="1:8">
+      <c r="I5" s="1">
+        <v>1.17</v>
+      </c>
+      <c r="J5" s="1">
+        <v>1.18</v>
+      </c>
+      <c r="K5" s="1">
+        <v>1.14</v>
+      </c>
+      <c r="L5" s="1">
+        <v>1.17</v>
+      </c>
+      <c r="M5" s="1">
+        <v>1.18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
       <c r="A6" s="1" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D6" s="1">
         <v>1.22</v>
@@ -1252,10 +1336,25 @@
       <c r="H6" s="1">
         <v>1.23</v>
       </c>
-    </row>
-    <row r="7" spans="2:8">
+      <c r="I6" s="1">
+        <v>1.23</v>
+      </c>
+      <c r="J6" s="1">
+        <v>1.23</v>
+      </c>
+      <c r="K6" s="1">
+        <v>1.23</v>
+      </c>
+      <c r="L6" s="1">
+        <v>1.22</v>
+      </c>
+      <c r="M6" s="1">
+        <v>1.22</v>
+      </c>
+    </row>
+    <row r="7" spans="2:13">
       <c r="B7" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D7" s="1">
         <v>0</v>
@@ -1272,10 +1371,25 @@
       <c r="H7" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="2:8">
+      <c r="I7" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="J7" s="1">
+        <v>0</v>
+      </c>
+      <c r="K7" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="L7" s="1">
+        <v>0</v>
+      </c>
+      <c r="M7" s="1">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="8" spans="2:13">
       <c r="B8" s="1" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D8" s="1">
         <v>1.22</v>
@@ -1292,13 +1406,28 @@
       <c r="H8" s="1">
         <v>1.23</v>
       </c>
-    </row>
-    <row r="9" spans="1:8">
+      <c r="I8" s="1">
+        <v>1.21</v>
+      </c>
+      <c r="J8" s="1">
+        <v>1.22</v>
+      </c>
+      <c r="K8" s="1">
+        <v>1.22</v>
+      </c>
+      <c r="L8" s="1">
+        <v>1.22</v>
+      </c>
+      <c r="M8" s="1">
+        <v>1.21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
       <c r="A9" s="1" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D9" s="1">
         <v>1.25</v>
@@ -1315,10 +1444,25 @@
       <c r="H9" s="1">
         <v>1.26</v>
       </c>
-    </row>
-    <row r="10" spans="2:8">
+      <c r="I9" s="1">
+        <v>1.25</v>
+      </c>
+      <c r="J9" s="1">
+        <v>1.26</v>
+      </c>
+      <c r="K9" s="1">
+        <v>1.26</v>
+      </c>
+      <c r="L9" s="1">
+        <v>1.26</v>
+      </c>
+      <c r="M9" s="1">
+        <v>1.26</v>
+      </c>
+    </row>
+    <row r="10" spans="2:13">
       <c r="B10" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D10" s="1">
         <v>0.06</v>
@@ -1335,10 +1479,25 @@
       <c r="H10" s="1">
         <v>0.04</v>
       </c>
-    </row>
-    <row r="11" spans="2:8">
+      <c r="I10" s="1">
+        <v>0.06</v>
+      </c>
+      <c r="J10" s="1">
+        <v>0.06</v>
+      </c>
+      <c r="K10" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="L10" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="M10" s="1">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="11" spans="2:13">
       <c r="B11" s="1" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D11" s="1">
         <v>1.19</v>
@@ -1355,13 +1514,28 @@
       <c r="H11" s="1">
         <v>1.21</v>
       </c>
-    </row>
-    <row r="12" spans="1:8">
+      <c r="I11" s="1">
+        <v>1.19</v>
+      </c>
+      <c r="J11" s="1">
+        <v>1.19</v>
+      </c>
+      <c r="K11" s="1">
+        <v>1.16</v>
+      </c>
+      <c r="L11" s="1">
+        <v>1.2</v>
+      </c>
+      <c r="M11" s="1">
+        <v>1.19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
       <c r="A12" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="D12" s="1">
         <v>1.26</v>
@@ -1378,10 +1552,25 @@
       <c r="H12" s="1">
         <v>1.26</v>
       </c>
-    </row>
-    <row r="13" spans="2:8">
+      <c r="I12" s="1">
+        <v>1.25</v>
+      </c>
+      <c r="J12" s="1">
+        <v>1.25</v>
+      </c>
+      <c r="K12" s="1">
+        <v>1.25</v>
+      </c>
+      <c r="L12" s="1">
+        <v>1.26</v>
+      </c>
+      <c r="M12" s="1">
+        <v>1.26</v>
+      </c>
+    </row>
+    <row r="13" spans="2:13">
       <c r="B13" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D13" s="1">
         <v>0.01</v>
@@ -1398,10 +1587,25 @@
       <c r="H13" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="2:8">
+      <c r="I13" s="1">
+        <v>0</v>
+      </c>
+      <c r="J13" s="1">
+        <v>0</v>
+      </c>
+      <c r="K13" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="L13" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="M13" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="2:13">
       <c r="B14" s="1" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D14" s="1">
         <v>1.24</v>
@@ -1418,13 +1622,28 @@
       <c r="H14" s="1">
         <v>1.26</v>
       </c>
-    </row>
-    <row r="15" spans="1:8">
+      <c r="I14" s="1">
+        <v>1.25</v>
+      </c>
+      <c r="J14" s="1">
+        <v>1.24</v>
+      </c>
+      <c r="K14" s="1">
+        <v>1.24</v>
+      </c>
+      <c r="L14" s="1">
+        <v>1.24</v>
+      </c>
+      <c r="M14" s="1">
+        <v>1.26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13">
       <c r="A15" s="1" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D15" s="1">
         <v>1.45</v>
@@ -1441,10 +1660,25 @@
       <c r="H15" s="1">
         <v>1.47</v>
       </c>
-    </row>
-    <row r="16" spans="2:8">
+      <c r="I15" s="1">
+        <v>1.45</v>
+      </c>
+      <c r="J15" s="1">
+        <v>1.46</v>
+      </c>
+      <c r="K15" s="1">
+        <v>1.46</v>
+      </c>
+      <c r="L15" s="1">
+        <v>1.45</v>
+      </c>
+      <c r="M15" s="1">
+        <v>1.45</v>
+      </c>
+    </row>
+    <row r="16" spans="2:13">
       <c r="B16" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D16" s="1">
         <v>0.1</v>
@@ -1461,10 +1695,25 @@
       <c r="H16" s="1">
         <v>0.12</v>
       </c>
-    </row>
-    <row r="17" spans="2:8">
+      <c r="I16" s="1">
+        <v>0.14</v>
+      </c>
+      <c r="J16" s="1">
+        <v>0.12</v>
+      </c>
+      <c r="K16" s="1">
+        <v>0.15</v>
+      </c>
+      <c r="L16" s="1">
+        <v>0.12</v>
+      </c>
+      <c r="M16" s="1">
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="17" spans="2:13">
       <c r="B17" s="1" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D17" s="1">
         <v>1.34</v>
@@ -1481,13 +1730,28 @@
       <c r="H17" s="1">
         <v>1.35</v>
       </c>
-    </row>
-    <row r="18" spans="1:8">
+      <c r="I17" s="1">
+        <v>1.31</v>
+      </c>
+      <c r="J17" s="1">
+        <v>1.34</v>
+      </c>
+      <c r="K17" s="1">
+        <v>1.3</v>
+      </c>
+      <c r="L17" s="1">
+        <v>1.33</v>
+      </c>
+      <c r="M17" s="1">
+        <v>1.34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13">
       <c r="A18" s="1" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D18" s="1">
         <v>1.33</v>
@@ -1504,10 +1768,25 @@
       <c r="H18" s="1">
         <v>1.34</v>
       </c>
-    </row>
-    <row r="19" spans="2:8">
+      <c r="I18" s="1">
+        <v>1.34</v>
+      </c>
+      <c r="J18" s="1">
+        <v>1.34</v>
+      </c>
+      <c r="K18" s="1">
+        <v>1.33</v>
+      </c>
+      <c r="L18" s="1">
+        <v>1.34</v>
+      </c>
+      <c r="M18" s="1">
+        <v>1.34</v>
+      </c>
+    </row>
+    <row r="19" spans="2:13">
       <c r="B19" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D19" s="1">
         <v>0.01</v>
@@ -1524,10 +1803,25 @@
       <c r="H19" s="1">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="20" spans="2:8">
+      <c r="I19" s="1">
+        <v>0.02</v>
+      </c>
+      <c r="J19" s="1">
+        <v>0.02</v>
+      </c>
+      <c r="K19" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="L19" s="1">
+        <v>0.02</v>
+      </c>
+      <c r="M19" s="1">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="20" spans="2:13">
       <c r="B20" s="1" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D20" s="1">
         <v>1.32</v>
@@ -1544,13 +1838,28 @@
       <c r="H20" s="1">
         <v>1.32</v>
       </c>
-    </row>
-    <row r="21" spans="1:8">
+      <c r="I20" s="1">
+        <v>1.32</v>
+      </c>
+      <c r="J20" s="1">
+        <v>1.32</v>
+      </c>
+      <c r="K20" s="1">
+        <v>1.32</v>
+      </c>
+      <c r="L20" s="1">
+        <v>1.31</v>
+      </c>
+      <c r="M20" s="1">
+        <v>1.32</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13">
       <c r="A21" s="1" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D21" s="1">
         <v>2.72</v>
@@ -1567,10 +1876,25 @@
       <c r="H21" s="1">
         <v>2.72</v>
       </c>
-    </row>
-    <row r="22" spans="2:8">
+      <c r="I21" s="1">
+        <v>2.71</v>
+      </c>
+      <c r="J21" s="1">
+        <v>2.79</v>
+      </c>
+      <c r="K21" s="1">
+        <v>2.72</v>
+      </c>
+      <c r="L21" s="1">
+        <v>2.72</v>
+      </c>
+      <c r="M21" s="1">
+        <v>2.72</v>
+      </c>
+    </row>
+    <row r="22" spans="2:13">
       <c r="B22" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D22" s="1">
         <v>0.01</v>
@@ -1587,10 +1911,25 @@
       <c r="H22" s="1">
         <v>0.02</v>
       </c>
-    </row>
-    <row r="23" spans="2:8">
+      <c r="I22" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="J22" s="1">
+        <v>0</v>
+      </c>
+      <c r="K22" s="1">
+        <v>0.03</v>
+      </c>
+      <c r="L22" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="M22" s="1">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="23" spans="2:13">
       <c r="B23" s="1" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D23" s="1">
         <v>2.7</v>
@@ -1607,13 +1946,28 @@
       <c r="H23" s="1">
         <v>2.69</v>
       </c>
-    </row>
-    <row r="24" spans="1:8">
+      <c r="I23" s="1">
+        <v>2.7</v>
+      </c>
+      <c r="J23" s="1">
+        <v>2.78</v>
+      </c>
+      <c r="K23" s="1">
+        <v>2.68</v>
+      </c>
+      <c r="L23" s="1">
+        <v>2.7</v>
+      </c>
+      <c r="M23" s="1">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13">
       <c r="A24" s="1" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D24" s="1">
         <v>2.91</v>
@@ -1630,10 +1984,25 @@
       <c r="H24" s="1">
         <v>2.91</v>
       </c>
-    </row>
-    <row r="25" spans="2:8">
+      <c r="I24" s="1">
+        <v>2.9</v>
+      </c>
+      <c r="J24" s="1">
+        <v>2.9</v>
+      </c>
+      <c r="K24" s="1">
+        <v>2.9</v>
+      </c>
+      <c r="L24" s="1">
+        <v>2.91</v>
+      </c>
+      <c r="M24" s="1">
+        <v>2.9</v>
+      </c>
+    </row>
+    <row r="25" spans="2:13">
       <c r="B25" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D25" s="1">
         <v>0.02</v>
@@ -1650,10 +2019,25 @@
       <c r="H25" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="2:8">
+      <c r="I25" s="1">
+        <v>0.02</v>
+      </c>
+      <c r="J25" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="K25" s="1">
+        <v>0</v>
+      </c>
+      <c r="L25" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="M25" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="2:13">
       <c r="B26" s="1" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D26" s="1">
         <v>2.88</v>
@@ -1670,13 +2054,28 @@
       <c r="H26" s="1">
         <v>2.9</v>
       </c>
-    </row>
-    <row r="27" spans="1:8">
+      <c r="I26" s="1">
+        <v>2.88</v>
+      </c>
+      <c r="J26" s="1">
+        <v>2.89</v>
+      </c>
+      <c r="K26" s="1">
+        <v>2.9</v>
+      </c>
+      <c r="L26" s="1">
+        <v>2.9</v>
+      </c>
+      <c r="M26" s="1">
+        <v>2.89</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13">
       <c r="A27" s="1" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D27" s="1">
         <v>3.54</v>
@@ -1693,10 +2092,25 @@
       <c r="H27" s="1">
         <v>3.55</v>
       </c>
-    </row>
-    <row r="28" spans="2:8">
+      <c r="I27" s="1">
+        <v>3.56</v>
+      </c>
+      <c r="J27" s="1">
+        <v>3.53</v>
+      </c>
+      <c r="K27" s="1">
+        <v>3.55</v>
+      </c>
+      <c r="L27" s="1">
+        <v>3.54</v>
+      </c>
+      <c r="M27" s="1">
+        <v>3.55</v>
+      </c>
+    </row>
+    <row r="28" spans="2:13">
       <c r="B28" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D28" s="1">
         <v>0.26</v>
@@ -1713,10 +2127,25 @@
       <c r="H28" s="1">
         <v>0.27</v>
       </c>
-    </row>
-    <row r="29" spans="2:8">
+      <c r="I28" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="J28" s="1">
+        <v>0.34</v>
+      </c>
+      <c r="K28" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="L28" s="1">
+        <v>0.32</v>
+      </c>
+      <c r="M28" s="1">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="29" spans="2:13">
       <c r="B29" s="1" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D29" s="1">
         <v>3.28</v>
@@ -1733,13 +2162,28 @@
       <c r="H29" s="1">
         <v>3.28</v>
       </c>
-    </row>
-    <row r="30" spans="1:8">
+      <c r="I29" s="1">
+        <v>3.26</v>
+      </c>
+      <c r="J29" s="1">
+        <v>3.19</v>
+      </c>
+      <c r="K29" s="1">
+        <v>3.24</v>
+      </c>
+      <c r="L29" s="1">
+        <v>3.22</v>
+      </c>
+      <c r="M29" s="1">
+        <v>3.25</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13">
       <c r="A30" s="1" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D30" s="1">
         <v>2.98</v>
@@ -1756,10 +2200,25 @@
       <c r="H30" s="1">
         <v>3.04</v>
       </c>
-    </row>
-    <row r="31" spans="2:8">
+      <c r="I30" s="1">
+        <v>3.01</v>
+      </c>
+      <c r="J30" s="1">
+        <v>2.98</v>
+      </c>
+      <c r="K30" s="1">
+        <v>2.99</v>
+      </c>
+      <c r="L30" s="1">
+        <v>2.98</v>
+      </c>
+      <c r="M30" s="1">
+        <v>2.96</v>
+      </c>
+    </row>
+    <row r="31" spans="2:13">
       <c r="B31" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D31" s="1">
         <v>0.01</v>
@@ -1776,10 +2235,25 @@
       <c r="H31" s="1">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="32" spans="2:8">
+      <c r="I31" s="1">
+        <v>0</v>
+      </c>
+      <c r="J31" s="1">
+        <v>0.02</v>
+      </c>
+      <c r="K31" s="1">
+        <v>0.02</v>
+      </c>
+      <c r="L31" s="1">
+        <v>0</v>
+      </c>
+      <c r="M31" s="1">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="32" spans="2:13">
       <c r="B32" s="1" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D32" s="1">
         <v>2.96</v>
@@ -1796,13 +2270,28 @@
       <c r="H32" s="1">
         <v>3.03</v>
       </c>
-    </row>
-    <row r="33" spans="1:8">
+      <c r="I32" s="1">
+        <v>3</v>
+      </c>
+      <c r="J32" s="1">
+        <v>2.96</v>
+      </c>
+      <c r="K32" s="1">
+        <v>2.96</v>
+      </c>
+      <c r="L32" s="1">
+        <v>2.97</v>
+      </c>
+      <c r="M32" s="1">
+        <v>2.95</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13">
       <c r="A33" s="1" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D33" s="1">
         <v>4.08</v>
@@ -1819,10 +2308,25 @@
       <c r="H33" s="1">
         <v>4.12</v>
       </c>
-    </row>
-    <row r="34" spans="2:8">
+      <c r="I33" s="1">
+        <v>4.09</v>
+      </c>
+      <c r="J33" s="1">
+        <v>4.05</v>
+      </c>
+      <c r="K33" s="1">
+        <v>4.06</v>
+      </c>
+      <c r="L33" s="1">
+        <v>4.05</v>
+      </c>
+      <c r="M33" s="1">
+        <v>4.06</v>
+      </c>
+    </row>
+    <row r="34" spans="2:13">
       <c r="B34" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D34" s="1">
         <v>0.43</v>
@@ -1839,10 +2343,25 @@
       <c r="H34" s="1">
         <v>0.38</v>
       </c>
-    </row>
-    <row r="35" spans="2:8">
+      <c r="I34" s="1">
+        <v>0.36</v>
+      </c>
+      <c r="J34" s="1">
+        <v>0.34</v>
+      </c>
+      <c r="K34" s="1">
+        <v>0.38</v>
+      </c>
+      <c r="L34" s="1">
+        <v>0.38</v>
+      </c>
+      <c r="M34" s="1">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="35" spans="2:13">
       <c r="B35" s="1" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D35" s="1">
         <v>3.65</v>
@@ -1859,13 +2378,28 @@
       <c r="H35" s="1">
         <v>3.74</v>
       </c>
-    </row>
-    <row r="36" spans="1:8">
+      <c r="I35" s="1">
+        <v>3.72</v>
+      </c>
+      <c r="J35" s="1">
+        <v>3.71</v>
+      </c>
+      <c r="K35" s="1">
+        <v>3.68</v>
+      </c>
+      <c r="L35" s="1">
+        <v>3.67</v>
+      </c>
+      <c r="M35" s="1">
+        <v>3.66</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13">
       <c r="A36" s="1" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D36" s="1">
         <v>3.39</v>
@@ -1882,10 +2416,25 @@
       <c r="H36" s="1">
         <v>3.38</v>
       </c>
-    </row>
-    <row r="37" spans="2:8">
+      <c r="I36" s="1">
+        <v>3.39</v>
+      </c>
+      <c r="J36" s="1">
+        <v>3.38</v>
+      </c>
+      <c r="K36" s="1">
+        <v>3.39</v>
+      </c>
+      <c r="L36" s="1">
+        <v>3.39</v>
+      </c>
+      <c r="M36" s="1">
+        <v>3.39</v>
+      </c>
+    </row>
+    <row r="37" spans="2:13">
       <c r="B37" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D37" s="1">
         <v>0.04</v>
@@ -1902,10 +2451,25 @@
       <c r="H37" s="1">
         <v>0.04</v>
       </c>
-    </row>
-    <row r="38" spans="2:8">
+      <c r="I37" s="1">
+        <v>0.06</v>
+      </c>
+      <c r="J37" s="1">
+        <v>0.04</v>
+      </c>
+      <c r="K37" s="1">
+        <v>0.04</v>
+      </c>
+      <c r="L37" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="M37" s="1">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="38" spans="2:13">
       <c r="B38" s="1" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D38" s="1">
         <v>3.35</v>
@@ -1922,13 +2486,28 @@
       <c r="H38" s="1">
         <v>3.34</v>
       </c>
-    </row>
-    <row r="39" spans="1:8">
+      <c r="I38" s="1">
+        <v>3.32</v>
+      </c>
+      <c r="J38" s="1">
+        <v>3.34</v>
+      </c>
+      <c r="K38" s="1">
+        <v>3.35</v>
+      </c>
+      <c r="L38" s="1">
+        <v>3.34</v>
+      </c>
+      <c r="M38" s="1">
+        <v>3.34</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13">
       <c r="A39" s="1" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D39" s="1">
         <v>9.03</v>
@@ -1945,10 +2524,25 @@
       <c r="H39" s="1">
         <v>8.94</v>
       </c>
-    </row>
-    <row r="40" spans="2:8">
+      <c r="I39" s="1">
+        <v>8.96</v>
+      </c>
+      <c r="J39" s="1">
+        <v>9.1</v>
+      </c>
+      <c r="K39" s="1">
+        <v>8.93</v>
+      </c>
+      <c r="L39" s="1">
+        <v>8.94</v>
+      </c>
+      <c r="M39" s="1">
+        <v>8.94</v>
+      </c>
+    </row>
+    <row r="40" spans="2:13">
       <c r="B40" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D40" s="1">
         <v>0.06</v>
@@ -1965,10 +2559,25 @@
       <c r="H40" s="1">
         <v>0.06</v>
       </c>
-    </row>
-    <row r="41" spans="2:8">
+      <c r="I40" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="J40" s="1">
+        <v>0.04</v>
+      </c>
+      <c r="K40" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="L40" s="1">
+        <v>0.08</v>
+      </c>
+      <c r="M40" s="1">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="41" spans="2:13">
       <c r="B41" s="1" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D41" s="1">
         <v>8.97</v>
@@ -1985,13 +2594,28 @@
       <c r="H41" s="1">
         <v>8.88</v>
       </c>
-    </row>
-    <row r="42" spans="1:8">
+      <c r="I41" s="1">
+        <v>8.91</v>
+      </c>
+      <c r="J41" s="1">
+        <v>9.06</v>
+      </c>
+      <c r="K41" s="1">
+        <v>8.88</v>
+      </c>
+      <c r="L41" s="1">
+        <v>8.86</v>
+      </c>
+      <c r="M41" s="1">
+        <v>8.88</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13">
       <c r="A42" s="1" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D42" s="1">
         <v>9.58</v>
@@ -2008,10 +2632,25 @@
       <c r="H42" s="1">
         <v>9.58</v>
       </c>
-    </row>
-    <row r="43" spans="2:8">
+      <c r="I42" s="1">
+        <v>9.59</v>
+      </c>
+      <c r="J42" s="1">
+        <v>9.61</v>
+      </c>
+      <c r="K42" s="1">
+        <v>9.6</v>
+      </c>
+      <c r="L42" s="1">
+        <v>9.61</v>
+      </c>
+      <c r="M42" s="1">
+        <v>9.63</v>
+      </c>
+    </row>
+    <row r="43" spans="2:13">
       <c r="B43" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D43" s="1">
         <v>0.04</v>
@@ -2028,10 +2667,25 @@
       <c r="H43" s="1">
         <v>0.04</v>
       </c>
-    </row>
-    <row r="44" spans="2:8">
+      <c r="I43" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="J43" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="K43" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="L43" s="1">
+        <v>0.03</v>
+      </c>
+      <c r="M43" s="1">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="44" spans="2:13">
       <c r="B44" s="1" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D44" s="1">
         <v>9.54</v>
@@ -2048,13 +2702,28 @@
       <c r="H44" s="1">
         <v>9.54</v>
       </c>
-    </row>
-    <row r="45" spans="1:8">
+      <c r="I44" s="1">
+        <v>9.54</v>
+      </c>
+      <c r="J44" s="1">
+        <v>9.56</v>
+      </c>
+      <c r="K44" s="1">
+        <v>9.59</v>
+      </c>
+      <c r="L44" s="1">
+        <v>9.58</v>
+      </c>
+      <c r="M44" s="1">
+        <v>9.61</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13">
       <c r="A45" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D45" s="1">
         <v>11.8</v>
@@ -2071,10 +2740,25 @@
       <c r="H45" s="1">
         <v>13.01</v>
       </c>
-    </row>
-    <row r="46" spans="2:8">
+      <c r="I45" s="1">
+        <v>11.8</v>
+      </c>
+      <c r="J45" s="1">
+        <v>11.82</v>
+      </c>
+      <c r="K45" s="1">
+        <v>11.8</v>
+      </c>
+      <c r="L45" s="1">
+        <v>11.77</v>
+      </c>
+      <c r="M45" s="1">
+        <v>11.79</v>
+      </c>
+    </row>
+    <row r="46" spans="2:13">
       <c r="B46" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D46" s="1">
         <v>0.92</v>
@@ -2091,10 +2775,25 @@
       <c r="H46" s="1">
         <v>0.82</v>
       </c>
-    </row>
-    <row r="47" spans="2:8">
+      <c r="I46" s="1">
+        <v>0.92</v>
+      </c>
+      <c r="J46" s="1">
+        <v>0.92</v>
+      </c>
+      <c r="K46" s="1">
+        <v>0.86</v>
+      </c>
+      <c r="L46" s="1">
+        <v>0.85</v>
+      </c>
+      <c r="M46" s="1">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="47" spans="2:13">
       <c r="B47" s="1" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D47" s="1">
         <v>10.89</v>
@@ -2111,13 +2810,28 @@
       <c r="H47" s="1">
         <v>12.19</v>
       </c>
-    </row>
-    <row r="48" spans="1:8">
+      <c r="I47" s="1">
+        <v>10.88</v>
+      </c>
+      <c r="J47" s="1">
+        <v>10.9</v>
+      </c>
+      <c r="K47" s="1">
+        <v>10.94</v>
+      </c>
+      <c r="L47" s="1">
+        <v>10.92</v>
+      </c>
+      <c r="M47" s="1">
+        <v>10.99</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13">
       <c r="A48" s="1" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D48" s="1">
         <v>10.79</v>
@@ -2134,10 +2848,25 @@
       <c r="H48" s="1">
         <v>10.92</v>
       </c>
-    </row>
-    <row r="49" spans="2:8">
+      <c r="I48" s="1">
+        <v>10.83</v>
+      </c>
+      <c r="J48" s="1">
+        <v>10.83</v>
+      </c>
+      <c r="K48" s="1">
+        <v>10.79</v>
+      </c>
+      <c r="L48" s="1">
+        <v>10.76</v>
+      </c>
+      <c r="M48" s="1">
+        <v>10.83</v>
+      </c>
+    </row>
+    <row r="49" spans="2:13">
       <c r="B49" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D49" s="1">
         <v>0.12</v>
@@ -2154,10 +2883,25 @@
       <c r="H49" s="1">
         <v>0.09</v>
       </c>
-    </row>
-    <row r="50" spans="2:8">
+      <c r="I49" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="J49" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="K49" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="L49" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="M49" s="1">
+        <v>10.83</v>
+      </c>
+    </row>
+    <row r="50" spans="2:13">
       <c r="B50" s="1" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D50" s="1">
         <v>10.67</v>
@@ -2174,13 +2918,28 @@
       <c r="H50" s="1">
         <v>10.83</v>
       </c>
-    </row>
-    <row r="51" spans="1:8">
+      <c r="I50" s="1">
+        <v>10.74</v>
+      </c>
+      <c r="J50" s="1">
+        <v>10.73</v>
+      </c>
+      <c r="K50" s="1">
+        <v>10.74</v>
+      </c>
+      <c r="L50" s="1">
+        <v>10.67</v>
+      </c>
+      <c r="M50" s="1">
+        <v>10.72</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13">
       <c r="A51" s="1" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D51" s="1">
         <v>15.38</v>
@@ -2197,10 +2956,25 @@
       <c r="H51" s="1">
         <v>16.65</v>
       </c>
-    </row>
-    <row r="52" spans="2:8">
+      <c r="I51" s="1">
+        <v>15.37</v>
+      </c>
+      <c r="J51" s="1">
+        <v>15.36</v>
+      </c>
+      <c r="K51" s="1">
+        <v>15.39</v>
+      </c>
+      <c r="L51" s="1">
+        <v>15.32</v>
+      </c>
+      <c r="M51" s="1">
+        <v>15.37</v>
+      </c>
+    </row>
+    <row r="52" spans="2:13">
       <c r="B52" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D52" s="1">
         <v>1.24</v>
@@ -2217,10 +2991,25 @@
       <c r="H52" s="1">
         <v>1.27</v>
       </c>
-    </row>
-    <row r="53" spans="2:8">
+      <c r="I52" s="1">
+        <v>1.22</v>
+      </c>
+      <c r="J52" s="1">
+        <v>1.11</v>
+      </c>
+      <c r="K52" s="1">
+        <v>1.16</v>
+      </c>
+      <c r="L52" s="1">
+        <v>1.16</v>
+      </c>
+      <c r="M52" s="1">
+        <v>1.12</v>
+      </c>
+    </row>
+    <row r="53" spans="2:13">
       <c r="B53" s="1" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D53" s="1">
         <v>12.68</v>
@@ -2237,13 +3026,28 @@
       <c r="H53" s="1">
         <v>13.93</v>
       </c>
-    </row>
-    <row r="54" spans="1:8">
+      <c r="I53" s="1">
+        <v>12.7</v>
+      </c>
+      <c r="J53" s="1">
+        <v>12.8</v>
+      </c>
+      <c r="K53" s="1">
+        <v>12.78</v>
+      </c>
+      <c r="L53" s="1">
+        <v>12.72</v>
+      </c>
+      <c r="M53" s="1">
+        <v>12.8</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13">
       <c r="A54" s="1" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D54" s="1">
         <v>13.1</v>
@@ -2260,10 +3064,25 @@
       <c r="H54" s="1">
         <v>13.05</v>
       </c>
-    </row>
-    <row r="55" spans="2:8">
+      <c r="I54" s="1">
+        <v>13.11</v>
+      </c>
+      <c r="J54" s="1">
+        <v>13.04</v>
+      </c>
+      <c r="K54" s="1">
+        <v>13.09</v>
+      </c>
+      <c r="L54" s="1">
+        <v>13.06</v>
+      </c>
+      <c r="M54" s="1">
+        <v>13.07</v>
+      </c>
+    </row>
+    <row r="55" spans="2:13">
       <c r="B55" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D55" s="1">
         <v>0.17</v>
@@ -2280,10 +3099,25 @@
       <c r="H55" s="1">
         <v>0.16</v>
       </c>
-    </row>
-    <row r="56" spans="2:8">
+      <c r="I55" s="1">
+        <v>0.16</v>
+      </c>
+      <c r="J55" s="1">
+        <v>0.14</v>
+      </c>
+      <c r="K55" s="1">
+        <v>0.19</v>
+      </c>
+      <c r="L55" s="1">
+        <v>0.18</v>
+      </c>
+      <c r="M55" s="1">
+        <v>0.14</v>
+      </c>
+    </row>
+    <row r="56" spans="2:13">
       <c r="B56" s="1" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D56" s="1">
         <v>11.48</v>
@@ -2300,13 +3134,28 @@
       <c r="H56" s="1">
         <v>11.44</v>
       </c>
-    </row>
-    <row r="57" spans="1:8">
+      <c r="I56" s="1">
+        <v>11.5</v>
+      </c>
+      <c r="J56" s="1">
+        <v>11.45</v>
+      </c>
+      <c r="K56" s="1">
+        <v>11.45</v>
+      </c>
+      <c r="L56" s="1">
+        <v>11.43</v>
+      </c>
+      <c r="M56" s="1">
+        <v>11.48</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13">
       <c r="A57" s="1" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D57" s="1">
         <v>43.61</v>
@@ -2323,10 +3172,25 @@
       <c r="H57" s="1">
         <v>44.36</v>
       </c>
-    </row>
-    <row r="58" spans="2:8">
+      <c r="I57" s="1">
+        <v>43.8</v>
+      </c>
+      <c r="J57" s="1">
+        <v>46.69</v>
+      </c>
+      <c r="K57" s="1">
+        <v>43.8</v>
+      </c>
+      <c r="L57" s="1">
+        <v>44.08</v>
+      </c>
+      <c r="M57" s="1">
+        <v>43.67</v>
+      </c>
+    </row>
+    <row r="58" spans="2:13">
       <c r="B58" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D58" s="1">
         <v>0.42</v>
@@ -2343,10 +3207,25 @@
       <c r="H58" s="1">
         <v>0.38</v>
       </c>
-    </row>
-    <row r="59" spans="2:8">
+      <c r="I58" s="1">
+        <v>0.38</v>
+      </c>
+      <c r="J58" s="1">
+        <v>0.44</v>
+      </c>
+      <c r="K58" s="1">
+        <v>0.38</v>
+      </c>
+      <c r="L58" s="1">
+        <v>0.42</v>
+      </c>
+      <c r="M58" s="1">
+        <v>0.39</v>
+      </c>
+    </row>
+    <row r="59" spans="2:13">
       <c r="B59" s="1" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D59" s="1">
         <v>43.2</v>
@@ -2363,13 +3242,28 @@
       <c r="H59" s="1">
         <v>43.99</v>
       </c>
-    </row>
-    <row r="60" spans="1:8">
+      <c r="I59" s="1">
+        <v>43.35</v>
+      </c>
+      <c r="J59" s="1">
+        <v>45.95</v>
+      </c>
+      <c r="K59" s="1">
+        <v>43.31</v>
+      </c>
+      <c r="L59" s="1">
+        <v>43.26</v>
+      </c>
+      <c r="M59" s="1">
+        <v>43.29</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13">
       <c r="A60" s="1" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D60" s="1">
         <v>46.39</v>
@@ -2386,10 +3280,25 @@
       <c r="H60" s="1">
         <v>46.4</v>
       </c>
-    </row>
-    <row r="61" spans="2:8">
+      <c r="I60" s="1">
+        <v>46.35</v>
+      </c>
+      <c r="J60" s="1">
+        <v>46.51</v>
+      </c>
+      <c r="K60" s="1">
+        <v>46.63</v>
+      </c>
+      <c r="L60" s="1">
+        <v>49.99</v>
+      </c>
+      <c r="M60" s="1">
+        <v>46.57</v>
+      </c>
+    </row>
+    <row r="61" spans="2:13">
       <c r="B61" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D61" s="1">
         <v>0.39</v>
@@ -2406,10 +3315,25 @@
       <c r="H61" s="1">
         <v>0.34</v>
       </c>
-    </row>
-    <row r="62" spans="2:8">
+      <c r="I61" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="J61" s="1">
+        <v>0.32</v>
+      </c>
+      <c r="K61" s="1">
+        <v>0.35</v>
+      </c>
+      <c r="L61" s="1">
+        <v>0.41</v>
+      </c>
+      <c r="M61" s="1">
+        <v>0.33</v>
+      </c>
+    </row>
+    <row r="62" spans="2:13">
       <c r="B62" s="1" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D62" s="1">
         <v>46.01</v>
@@ -2426,13 +3350,28 @@
       <c r="H62" s="1">
         <v>46.08</v>
       </c>
-    </row>
-    <row r="63" spans="1:8">
+      <c r="I62" s="1">
+        <v>46.07</v>
+      </c>
+      <c r="J62" s="1">
+        <v>46.2</v>
+      </c>
+      <c r="K62" s="1">
+        <v>46.3</v>
+      </c>
+      <c r="L62" s="1">
+        <v>49.59</v>
+      </c>
+      <c r="M62" s="1">
+        <v>46.25</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13">
       <c r="A63" s="1" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D63" s="1">
         <v>43.91</v>
@@ -2449,10 +3388,25 @@
       <c r="H63" s="1">
         <v>45.38</v>
       </c>
-    </row>
-    <row r="64" spans="2:8">
+      <c r="I63" s="1">
+        <v>44.04</v>
+      </c>
+      <c r="J63" s="1">
+        <v>44.26</v>
+      </c>
+      <c r="K63" s="1">
+        <v>44.22</v>
+      </c>
+      <c r="L63" s="1">
+        <v>47.29</v>
+      </c>
+      <c r="M63" s="1">
+        <v>44.01</v>
+      </c>
+    </row>
+    <row r="64" spans="2:13">
       <c r="B64" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D64" s="1">
         <v>0.29</v>
@@ -2469,10 +3423,25 @@
       <c r="H64" s="1">
         <v>0.33</v>
       </c>
-    </row>
-    <row r="65" spans="2:8">
+      <c r="I64" s="1">
+        <v>0.34</v>
+      </c>
+      <c r="J64" s="1">
+        <v>0.33</v>
+      </c>
+      <c r="K64" s="1">
+        <v>0.33</v>
+      </c>
+      <c r="L64" s="1">
+        <v>0.38</v>
+      </c>
+      <c r="M64" s="1">
+        <v>0.34</v>
+      </c>
+    </row>
+    <row r="65" spans="2:13">
       <c r="B65" s="1" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D65" s="1">
         <v>43.63</v>
@@ -2489,13 +3458,28 @@
       <c r="H65" s="1">
         <v>45.07</v>
       </c>
-    </row>
-    <row r="66" spans="1:8">
+      <c r="I65" s="1">
+        <v>43.72</v>
+      </c>
+      <c r="J65" s="1">
+        <v>43.95</v>
+      </c>
+      <c r="K65" s="1">
+        <v>43.9</v>
+      </c>
+      <c r="L65" s="1">
+        <v>46.92</v>
+      </c>
+      <c r="M65" s="1">
+        <v>43.69</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13">
       <c r="A66" s="1" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D66" s="1">
         <v>46.85</v>
@@ -2512,10 +3496,25 @@
       <c r="H66" s="1">
         <v>47.71</v>
       </c>
-    </row>
-    <row r="67" spans="2:8">
+      <c r="I66" s="1">
+        <v>46.95</v>
+      </c>
+      <c r="J66" s="1">
+        <v>46.91</v>
+      </c>
+      <c r="K66" s="1">
+        <v>46.91</v>
+      </c>
+      <c r="L66" s="1">
+        <v>47.48</v>
+      </c>
+      <c r="M66" s="1">
+        <v>46.89</v>
+      </c>
+    </row>
+    <row r="67" spans="2:13">
       <c r="B67" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D67" s="1">
         <v>0.34</v>
@@ -2532,10 +3531,25 @@
       <c r="H67" s="1">
         <v>0.35</v>
       </c>
-    </row>
-    <row r="68" spans="2:8">
+      <c r="I67" s="1">
+        <v>0.33</v>
+      </c>
+      <c r="J67" s="1">
+        <v>0.34</v>
+      </c>
+      <c r="K67" s="1">
+        <v>0.33</v>
+      </c>
+      <c r="L67" s="1">
+        <v>0.34</v>
+      </c>
+      <c r="M67" s="1">
+        <v>0.37</v>
+      </c>
+    </row>
+    <row r="68" spans="2:13">
       <c r="B68" s="1" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D68" s="1">
         <v>46.52</v>
@@ -2552,13 +3566,28 @@
       <c r="H68" s="1">
         <v>47.37</v>
       </c>
-    </row>
-    <row r="69" spans="1:8">
+      <c r="I68" s="1">
+        <v>46.64</v>
+      </c>
+      <c r="J68" s="1">
+        <v>46.58</v>
+      </c>
+      <c r="K68" s="1">
+        <v>46.6</v>
+      </c>
+      <c r="L68" s="1">
+        <v>47.15</v>
+      </c>
+      <c r="M68" s="1">
+        <v>46.54</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13">
       <c r="A69" s="1" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D69" s="1">
         <v>46.87</v>
@@ -2575,10 +3604,25 @@
       <c r="H69" s="1">
         <v>46.67</v>
       </c>
-    </row>
-    <row r="70" spans="2:8">
+      <c r="I69" s="1">
+        <v>46.7</v>
+      </c>
+      <c r="J69" s="1">
+        <v>46.74</v>
+      </c>
+      <c r="K69" s="1">
+        <v>46.85</v>
+      </c>
+      <c r="L69" s="1">
+        <v>49.62</v>
+      </c>
+      <c r="M69" s="1">
+        <v>47.01</v>
+      </c>
+    </row>
+    <row r="70" spans="2:13">
       <c r="B70" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D70" s="1">
         <v>0.72</v>
@@ -2595,10 +3639,25 @@
       <c r="H70" s="1">
         <v>0.82</v>
       </c>
-    </row>
-    <row r="71" spans="2:8">
+      <c r="I70" s="1">
+        <v>0.69</v>
+      </c>
+      <c r="J70" s="1">
+        <v>0.66</v>
+      </c>
+      <c r="K70" s="1">
+        <v>0.72</v>
+      </c>
+      <c r="L70" s="1">
+        <v>0.72</v>
+      </c>
+      <c r="M70" s="1">
+        <v>0.58</v>
+      </c>
+    </row>
+    <row r="71" spans="2:13">
       <c r="B71" s="1" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D71" s="1">
         <v>45.18</v>
@@ -2615,13 +3674,28 @@
       <c r="H71" s="1">
         <v>44.88</v>
       </c>
-    </row>
-    <row r="72" spans="1:8">
+      <c r="I71" s="1">
+        <v>45.04</v>
+      </c>
+      <c r="J71" s="1">
+        <v>45.12</v>
+      </c>
+      <c r="K71" s="1">
+        <v>45.16</v>
+      </c>
+      <c r="L71" s="1">
+        <v>47.93</v>
+      </c>
+      <c r="M71" s="1">
+        <v>45.46</v>
+      </c>
+    </row>
+    <row r="72" spans="1:13">
       <c r="A72" s="1" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D72" s="1">
         <v>52.08</v>
@@ -2638,10 +3712,25 @@
       <c r="H72" s="1">
         <v>49.77</v>
       </c>
-    </row>
-    <row r="73" spans="2:8">
+      <c r="I72" s="1">
+        <v>49.02</v>
+      </c>
+      <c r="J72" s="1">
+        <v>49.28</v>
+      </c>
+      <c r="K72" s="1">
+        <v>49.26</v>
+      </c>
+      <c r="L72" s="1">
+        <v>48.64</v>
+      </c>
+      <c r="M72" s="1">
+        <v>48.97</v>
+      </c>
+    </row>
+    <row r="73" spans="2:13">
       <c r="B73" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D73" s="1">
         <v>0.38</v>
@@ -2658,10 +3747,25 @@
       <c r="H73" s="1">
         <v>0.34</v>
       </c>
-    </row>
-    <row r="74" spans="2:8">
+      <c r="I73" s="1">
+        <v>0.33</v>
+      </c>
+      <c r="J73" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="K73" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="L73" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="M73" s="1">
+        <v>0.34</v>
+      </c>
+    </row>
+    <row r="74" spans="2:13">
       <c r="B74" s="1" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D74" s="1">
         <v>50.72</v>
@@ -2678,13 +3782,28 @@
       <c r="H74" s="1">
         <v>48.46</v>
       </c>
-    </row>
-    <row r="75" spans="1:8">
+      <c r="I74" s="1">
+        <v>47.72</v>
+      </c>
+      <c r="J74" s="1">
+        <v>48.01</v>
+      </c>
+      <c r="K74" s="1">
+        <v>47.99</v>
+      </c>
+      <c r="L74" s="1">
+        <v>47.38</v>
+      </c>
+      <c r="M74" s="1">
+        <v>47.66</v>
+      </c>
+    </row>
+    <row r="75" spans="1:13">
       <c r="A75" s="1" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D75" s="1">
         <v>1453.51</v>
@@ -2701,10 +3820,25 @@
       <c r="H75" s="1">
         <v>1463.12</v>
       </c>
-    </row>
-    <row r="76" spans="2:8">
+      <c r="I75" s="1">
+        <v>1446.99</v>
+      </c>
+      <c r="J75" s="1">
+        <v>1604.67</v>
+      </c>
+      <c r="K75" s="1">
+        <v>1453.79</v>
+      </c>
+      <c r="L75" s="1">
+        <v>1448.03</v>
+      </c>
+      <c r="M75" s="1">
+        <v>1444.87</v>
+      </c>
+    </row>
+    <row r="76" spans="2:13">
       <c r="B76" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D76" s="1">
         <v>12.54</v>
@@ -2721,10 +3855,25 @@
       <c r="H76" s="1">
         <v>12.95</v>
       </c>
-    </row>
-    <row r="77" spans="2:8">
+      <c r="I76" s="1">
+        <v>12.48</v>
+      </c>
+      <c r="J76" s="1">
+        <v>13.69</v>
+      </c>
+      <c r="K76" s="1">
+        <v>13.14</v>
+      </c>
+      <c r="L76" s="1">
+        <v>13.2</v>
+      </c>
+      <c r="M76" s="1">
+        <v>12.69</v>
+      </c>
+    </row>
+    <row r="77" spans="2:13">
       <c r="B77" s="1" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D77" s="1">
         <v>1441.8</v>
@@ -2741,13 +3890,28 @@
       <c r="H77" s="1">
         <v>1450.82</v>
       </c>
-    </row>
-    <row r="78" spans="1:8">
+      <c r="I77" s="1">
+        <v>1434.89</v>
+      </c>
+      <c r="J77" s="1">
+        <v>1591.46</v>
+      </c>
+      <c r="K77" s="1">
+        <v>1441.46</v>
+      </c>
+      <c r="L77" s="1">
+        <v>1434.49</v>
+      </c>
+      <c r="M77" s="1">
+        <v>1432.64</v>
+      </c>
+    </row>
+    <row r="78" spans="1:13">
       <c r="A78" s="1" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D78" s="1">
         <v>1546.07</v>
@@ -2764,10 +3928,25 @@
       <c r="H78" s="1">
         <v>1697.18</v>
       </c>
-    </row>
-    <row r="79" spans="2:8">
+      <c r="I78" s="1">
+        <v>1557.11</v>
+      </c>
+      <c r="J78" s="1">
+        <v>1690.9</v>
+      </c>
+      <c r="K78" s="1">
+        <v>1552.04</v>
+      </c>
+      <c r="L78" s="1">
+        <v>1542.5</v>
+      </c>
+      <c r="M78" s="1">
+        <v>1536.45</v>
+      </c>
+    </row>
+    <row r="79" spans="2:13">
       <c r="B79" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D79" s="1">
         <v>13.25</v>
@@ -2784,10 +3963,25 @@
       <c r="H79" s="1">
         <v>14.33</v>
       </c>
-    </row>
-    <row r="80" spans="2:8">
+      <c r="I79" s="1">
+        <v>13.44</v>
+      </c>
+      <c r="J79" s="1">
+        <v>14.03</v>
+      </c>
+      <c r="K79" s="1">
+        <v>13.16</v>
+      </c>
+      <c r="L79" s="1">
+        <v>13.24</v>
+      </c>
+      <c r="M79" s="1">
+        <v>13.09</v>
+      </c>
+    </row>
+    <row r="80" spans="2:13">
       <c r="B80" s="1" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D80" s="1">
         <v>1533.74</v>
@@ -2804,13 +3998,28 @@
       <c r="H80" s="1">
         <v>1683.16</v>
       </c>
-    </row>
-    <row r="81" spans="1:8">
+      <c r="I80" s="1">
+        <v>1544.57</v>
+      </c>
+      <c r="J80" s="1">
+        <v>1677.16</v>
+      </c>
+      <c r="K80" s="1">
+        <v>1539.08</v>
+      </c>
+      <c r="L80" s="1">
+        <v>1529.33</v>
+      </c>
+      <c r="M80" s="1">
+        <v>1523.76</v>
+      </c>
+    </row>
+    <row r="81" spans="1:13">
       <c r="A81" s="1" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D81" s="1">
         <v>1473.22</v>
@@ -2827,10 +4036,25 @@
       <c r="H81" s="1">
         <v>1559.15</v>
       </c>
-    </row>
-    <row r="82" spans="2:8">
+      <c r="I81" s="1">
+        <v>1481.37</v>
+      </c>
+      <c r="J81" s="1">
+        <v>1558.57</v>
+      </c>
+      <c r="K81" s="5">
+        <v>2271.6</v>
+      </c>
+      <c r="L81" s="1">
+        <v>1464.43</v>
+      </c>
+      <c r="M81" s="1">
+        <v>1471.31</v>
+      </c>
+    </row>
+    <row r="82" spans="2:13">
       <c r="B82" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D82" s="1">
         <v>13.2</v>
@@ -2847,10 +4071,25 @@
       <c r="H82" s="1">
         <v>13.87</v>
       </c>
-    </row>
-    <row r="83" spans="2:8">
+      <c r="I82" s="1">
+        <v>13.2</v>
+      </c>
+      <c r="J82" s="1">
+        <v>13.62</v>
+      </c>
+      <c r="K82" s="1">
+        <v>16.89</v>
+      </c>
+      <c r="L82" s="1">
+        <v>13.4</v>
+      </c>
+      <c r="M82" s="1">
+        <v>13.15</v>
+      </c>
+    </row>
+    <row r="83" spans="2:13">
       <c r="B83" s="1" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D83" s="1">
         <v>1460.88</v>
@@ -2867,13 +4106,28 @@
       <c r="H83" s="1">
         <v>1545.96</v>
       </c>
-    </row>
-    <row r="84" spans="1:8">
+      <c r="I83" s="1">
+        <v>1468.33</v>
+      </c>
+      <c r="J83" s="1">
+        <v>1544.04</v>
+      </c>
+      <c r="K83" s="1">
+        <v>1607.88</v>
+      </c>
+      <c r="L83" s="1">
+        <v>1451.65</v>
+      </c>
+      <c r="M83" s="1">
+        <v>1458.31</v>
+      </c>
+    </row>
+    <row r="84" spans="1:13">
       <c r="A84" s="1" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D84" s="1">
         <v>1555.73</v>
@@ -2890,10 +4144,25 @@
       <c r="H84" s="1">
         <v>1700.78</v>
       </c>
-    </row>
-    <row r="85" spans="2:8">
+      <c r="I84" s="1">
+        <v>1549</v>
+      </c>
+      <c r="J84" s="1">
+        <v>1670.27</v>
+      </c>
+      <c r="K84" s="1">
+        <v>1765.28</v>
+      </c>
+      <c r="L84" s="1">
+        <v>1567.22</v>
+      </c>
+      <c r="M84" s="1">
+        <v>1563.34</v>
+      </c>
+    </row>
+    <row r="85" spans="2:13">
       <c r="B85" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D85" s="1">
         <v>13.26</v>
@@ -2910,10 +4179,25 @@
       <c r="H85" s="1">
         <v>13.85</v>
       </c>
-    </row>
-    <row r="86" spans="2:8">
+      <c r="I85" s="1">
+        <v>13.43</v>
+      </c>
+      <c r="J85" s="1">
+        <v>13.65</v>
+      </c>
+      <c r="K85" s="1">
+        <v>14.13</v>
+      </c>
+      <c r="L85" s="1">
+        <v>13.34</v>
+      </c>
+      <c r="M85" s="1">
+        <v>13.2</v>
+      </c>
+    </row>
+    <row r="86" spans="2:13">
       <c r="B86" s="1" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D86" s="1">
         <v>1543.38</v>
@@ -2930,13 +4214,28 @@
       <c r="H86" s="1">
         <v>1687.74</v>
       </c>
-    </row>
-    <row r="87" spans="1:8">
+      <c r="I86" s="1">
+        <v>1535.97</v>
+      </c>
+      <c r="J86" s="1">
+        <v>1657.06</v>
+      </c>
+      <c r="K86" s="1">
+        <v>1579.3</v>
+      </c>
+      <c r="L86" s="1">
+        <v>1554.53</v>
+      </c>
+      <c r="M86" s="1">
+        <v>1550.5</v>
+      </c>
+    </row>
+    <row r="87" spans="1:13">
       <c r="A87" s="1" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D87" s="1">
         <v>2754.5</v>
@@ -2953,10 +4252,25 @@
       <c r="H87" s="1">
         <v>2996.95</v>
       </c>
-    </row>
-    <row r="88" spans="2:8">
+      <c r="I87" s="1">
+        <v>2760.54</v>
+      </c>
+      <c r="J87" s="1">
+        <v>3044.56</v>
+      </c>
+      <c r="K87" s="1">
+        <v>2772.51</v>
+      </c>
+      <c r="L87" s="1">
+        <v>2766.79</v>
+      </c>
+      <c r="M87" s="1">
+        <v>2767.22</v>
+      </c>
+    </row>
+    <row r="88" spans="2:13">
       <c r="B88" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D88" s="1">
         <v>27.03</v>
@@ -2973,10 +4287,25 @@
       <c r="H88" s="1">
         <v>28.05</v>
       </c>
-    </row>
-    <row r="89" spans="2:8">
+      <c r="I88" s="1">
+        <v>27.04</v>
+      </c>
+      <c r="J88" s="1">
+        <v>27.57</v>
+      </c>
+      <c r="K88" s="1">
+        <v>26.61</v>
+      </c>
+      <c r="L88" s="1">
+        <v>26.28</v>
+      </c>
+      <c r="M88" s="1">
+        <v>27.42</v>
+      </c>
+    </row>
+    <row r="89" spans="2:13">
       <c r="B89" s="1" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D89" s="1">
         <v>2716.71</v>
@@ -2993,13 +4322,28 @@
       <c r="H89" s="1">
         <v>2957.4</v>
       </c>
-    </row>
-    <row r="90" spans="1:8">
+      <c r="I89" s="1">
+        <v>2721.28</v>
+      </c>
+      <c r="J89" s="1">
+        <v>3004.46</v>
+      </c>
+      <c r="K89" s="1">
+        <v>2720.23</v>
+      </c>
+      <c r="L89" s="1">
+        <v>2728.15</v>
+      </c>
+      <c r="M89" s="1">
+        <v>2726.32</v>
+      </c>
+    </row>
+    <row r="90" spans="1:13">
       <c r="A90" s="1" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D90" s="1">
         <v>3058.42</v>
@@ -3016,10 +4360,25 @@
       <c r="H90" s="1">
         <v>3153.66</v>
       </c>
-    </row>
-    <row r="91" spans="2:8">
+      <c r="I90" s="1">
+        <v>3061.27</v>
+      </c>
+      <c r="J90" s="1">
+        <v>3373.23</v>
+      </c>
+      <c r="K90" s="1">
+        <v>3053.72</v>
+      </c>
+      <c r="L90" s="1">
+        <v>3047.07</v>
+      </c>
+      <c r="M90" s="1">
+        <v>3049.79</v>
+      </c>
+    </row>
+    <row r="91" spans="2:13">
       <c r="B91" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D91" s="1">
         <v>26.69</v>
@@ -3036,10 +4395,25 @@
       <c r="H91" s="1">
         <v>27.15</v>
       </c>
-    </row>
-    <row r="92" spans="2:8">
+      <c r="I91" s="1">
+        <v>26.72</v>
+      </c>
+      <c r="J91" s="1">
+        <v>28.86</v>
+      </c>
+      <c r="K91" s="1">
+        <v>26.33</v>
+      </c>
+      <c r="L91" s="1">
+        <v>27.16</v>
+      </c>
+      <c r="M91" s="1">
+        <v>26.91</v>
+      </c>
+    </row>
+    <row r="92" spans="2:13">
       <c r="B92" s="1" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D92" s="1">
         <v>3021.22</v>
@@ -3056,13 +4430,28 @@
       <c r="H92" s="1">
         <v>3115.86</v>
       </c>
-    </row>
-    <row r="93" spans="1:8">
+      <c r="I92" s="1">
+        <v>3022.46</v>
+      </c>
+      <c r="J92" s="1">
+        <v>3330.62</v>
+      </c>
+      <c r="K92" s="1">
+        <v>3015.16</v>
+      </c>
+      <c r="L92" s="1">
+        <v>3008.53</v>
+      </c>
+      <c r="M92" s="1">
+        <v>3011.96</v>
+      </c>
+    </row>
+    <row r="93" spans="1:13">
       <c r="A93" s="1" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D93" s="1">
         <v>1528.61</v>
@@ -3079,10 +4468,25 @@
       <c r="H93" s="1">
         <v>1580.35</v>
       </c>
-    </row>
-    <row r="94" spans="2:8">
+      <c r="I93" s="1">
+        <v>1568.74</v>
+      </c>
+      <c r="J93" s="1">
+        <v>1644.14</v>
+      </c>
+      <c r="K93" s="1">
+        <v>1542.47</v>
+      </c>
+      <c r="L93" s="1">
+        <v>1555.08</v>
+      </c>
+      <c r="M93" s="1">
+        <v>1546.09</v>
+      </c>
+    </row>
+    <row r="94" spans="2:13">
       <c r="B94" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D94" s="1">
         <v>14.18</v>
@@ -3099,10 +4503,25 @@
       <c r="H94" s="1">
         <v>14.12</v>
       </c>
-    </row>
-    <row r="95" spans="2:8">
+      <c r="I94" s="1">
+        <v>15.27</v>
+      </c>
+      <c r="J94" s="1">
+        <v>15.91</v>
+      </c>
+      <c r="K94" s="1">
+        <v>14.64</v>
+      </c>
+      <c r="L94" s="1">
+        <v>14.5</v>
+      </c>
+      <c r="M94" s="1">
+        <v>14.45</v>
+      </c>
+    </row>
+    <row r="95" spans="2:13">
       <c r="B95" s="1" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D95" s="1">
         <v>1515.3</v>
@@ -3119,13 +4538,28 @@
       <c r="H95" s="1">
         <v>1567.14</v>
       </c>
-    </row>
-    <row r="96" spans="1:8">
+      <c r="I95" s="1">
+        <v>1554.35</v>
+      </c>
+      <c r="J95" s="1">
+        <v>1629.16</v>
+      </c>
+      <c r="K95" s="1">
+        <v>1528.46</v>
+      </c>
+      <c r="L95" s="1">
+        <v>1541.47</v>
+      </c>
+      <c r="M95" s="1">
+        <v>1532.19</v>
+      </c>
+    </row>
+    <row r="96" spans="1:13">
       <c r="A96" s="1" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D96" s="1">
         <v>1586.76</v>
@@ -3142,10 +4576,25 @@
       <c r="H96" s="1">
         <v>1645.97</v>
       </c>
-    </row>
-    <row r="97" spans="2:8">
+      <c r="I96" s="1">
+        <v>1623.72</v>
+      </c>
+      <c r="J96" s="1">
+        <v>1609.65</v>
+      </c>
+      <c r="K96" s="1">
+        <v>1609.68</v>
+      </c>
+      <c r="L96" s="1">
+        <v>1616.45</v>
+      </c>
+      <c r="M96" s="1">
+        <v>1588.07</v>
+      </c>
+    </row>
+    <row r="97" spans="2:13">
       <c r="B97" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D97" s="1">
         <v>14.51</v>
@@ -3162,10 +4611,25 @@
       <c r="H97" s="1">
         <v>14.68</v>
       </c>
-    </row>
-    <row r="98" spans="2:8">
+      <c r="I97" s="1">
+        <v>15.33</v>
+      </c>
+      <c r="J97" s="1">
+        <v>14.53</v>
+      </c>
+      <c r="K97" s="1">
+        <v>15.08</v>
+      </c>
+      <c r="L97" s="1">
+        <v>14.92</v>
+      </c>
+      <c r="M97" s="1">
+        <v>14.82</v>
+      </c>
+    </row>
+    <row r="98" spans="2:13">
       <c r="B98" s="1" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D98" s="1">
         <v>1573.16</v>
@@ -3182,13 +4646,28 @@
       <c r="H98" s="1">
         <v>1632.22</v>
       </c>
-    </row>
-    <row r="99" spans="1:8">
+      <c r="I98" s="1">
+        <v>1609.28</v>
+      </c>
+      <c r="J98" s="1">
+        <v>1596.04</v>
+      </c>
+      <c r="K98" s="1">
+        <v>1595.03</v>
+      </c>
+      <c r="L98" s="1">
+        <v>1602.44</v>
+      </c>
+      <c r="M98" s="1">
+        <v>1574.14</v>
+      </c>
+    </row>
+    <row r="99" spans="1:13">
       <c r="A99" s="1" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D99" s="1">
         <v>1575.98</v>
@@ -3205,10 +4684,25 @@
       <c r="H99" s="1">
         <v>1567.74</v>
       </c>
-    </row>
-    <row r="100" spans="2:8">
+      <c r="I99" s="1">
+        <v>1600.67</v>
+      </c>
+      <c r="J99" s="1">
+        <v>1580.54</v>
+      </c>
+      <c r="K99" s="5">
+        <v>2438.5</v>
+      </c>
+      <c r="L99" s="1">
+        <v>1560.45</v>
+      </c>
+      <c r="M99" s="1">
+        <v>1564.92</v>
+      </c>
+    </row>
+    <row r="100" spans="2:13">
       <c r="B100" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D100" s="1">
         <v>15.93</v>
@@ -3225,10 +4719,25 @@
       <c r="H100" s="1">
         <v>15.43</v>
       </c>
-    </row>
-    <row r="101" spans="2:8">
+      <c r="I100" s="1">
+        <v>15.31</v>
+      </c>
+      <c r="J100" s="1">
+        <v>15.81</v>
+      </c>
+      <c r="K100" s="1">
+        <v>20.03</v>
+      </c>
+      <c r="L100" s="1">
+        <v>15.55</v>
+      </c>
+      <c r="M100" s="1">
+        <v>15.27</v>
+      </c>
+    </row>
+    <row r="101" spans="2:13">
       <c r="B101" s="1" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D101" s="1">
         <v>1560.93</v>
@@ -3245,13 +4754,28 @@
       <c r="H101" s="1">
         <v>1553.17</v>
       </c>
-    </row>
-    <row r="102" spans="1:8">
+      <c r="I101" s="1">
+        <v>1586.23</v>
+      </c>
+      <c r="J101" s="1">
+        <v>1565.62</v>
+      </c>
+      <c r="K101" s="1">
+        <v>1749.73</v>
+      </c>
+      <c r="L101" s="1">
+        <v>1545.77</v>
+      </c>
+      <c r="M101" s="1">
+        <v>1550.51</v>
+      </c>
+    </row>
+    <row r="102" spans="1:13">
       <c r="A102" s="1" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D102" s="1">
         <v>1622.35</v>
@@ -3268,10 +4792,25 @@
       <c r="H102" s="1">
         <v>1639.4</v>
       </c>
-    </row>
-    <row r="103" spans="2:8">
+      <c r="I102" s="1">
+        <v>1666.86</v>
+      </c>
+      <c r="J102" s="1">
+        <v>1808.76</v>
+      </c>
+      <c r="K102" s="5">
+        <v>1901.74</v>
+      </c>
+      <c r="L102" s="1">
+        <v>1659.3</v>
+      </c>
+      <c r="M102" s="1">
+        <v>1638.1</v>
+      </c>
+    </row>
+    <row r="103" spans="2:13">
       <c r="B103" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D103" s="1">
         <v>14.82</v>
@@ -3288,10 +4827,25 @@
       <c r="H103" s="1">
         <v>14.46</v>
       </c>
-    </row>
-    <row r="104" spans="2:8">
+      <c r="I103" s="1">
+        <v>15.76</v>
+      </c>
+      <c r="J103" s="1">
+        <v>15.93</v>
+      </c>
+      <c r="K103" s="1">
+        <v>16.25</v>
+      </c>
+      <c r="L103" s="1">
+        <v>15.2</v>
+      </c>
+      <c r="M103" s="1">
+        <v>15.22</v>
+      </c>
+    </row>
+    <row r="104" spans="2:13">
       <c r="B104" s="1" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D104" s="1">
         <v>1608.43</v>
@@ -3308,13 +4862,28 @@
       <c r="H104" s="1">
         <v>1625.83</v>
       </c>
-    </row>
-    <row r="105" spans="1:8">
+      <c r="I104" s="1">
+        <v>1652.01</v>
+      </c>
+      <c r="J104" s="1">
+        <v>1793.84</v>
+      </c>
+      <c r="K104" s="1">
+        <v>1700.57</v>
+      </c>
+      <c r="L104" s="1">
+        <v>1644.84</v>
+      </c>
+      <c r="M104" s="1">
+        <v>1623.61</v>
+      </c>
+    </row>
+    <row r="105" spans="1:13">
       <c r="A105" s="1" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D105" s="1">
         <v>2734.07</v>
@@ -3331,10 +4900,25 @@
       <c r="H105" s="1">
         <v>2791.15</v>
       </c>
-    </row>
-    <row r="106" spans="2:8">
+      <c r="I105" s="1">
+        <v>2734.76</v>
+      </c>
+      <c r="J105" s="1">
+        <v>3023.91</v>
+      </c>
+      <c r="K105" s="1">
+        <v>2750.71</v>
+      </c>
+      <c r="L105" s="1">
+        <v>2727.14</v>
+      </c>
+      <c r="M105" s="1">
+        <v>2733.88</v>
+      </c>
+    </row>
+    <row r="106" spans="2:13">
       <c r="B106" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D106" s="1">
         <v>28.71</v>
@@ -3351,10 +4935,25 @@
       <c r="H106" s="1">
         <v>29.44</v>
       </c>
-    </row>
-    <row r="107" spans="2:8">
+      <c r="I106" s="1">
+        <v>28.97</v>
+      </c>
+      <c r="J106" s="1">
+        <v>31.08</v>
+      </c>
+      <c r="K106" s="1">
+        <v>29.26</v>
+      </c>
+      <c r="L106" s="1">
+        <v>28.76</v>
+      </c>
+      <c r="M106" s="1">
+        <v>29.04</v>
+      </c>
+    </row>
+    <row r="107" spans="2:13">
       <c r="B107" s="1" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D107" s="1">
         <v>2703.42</v>
@@ -3371,13 +4970,28 @@
       <c r="H107" s="1">
         <v>2759.75</v>
       </c>
-    </row>
-    <row r="108" spans="1:8">
+      <c r="I107" s="1">
+        <v>2703.79</v>
+      </c>
+      <c r="J107" s="1">
+        <v>2991.03</v>
+      </c>
+      <c r="K107" s="1">
+        <v>2707.34</v>
+      </c>
+      <c r="L107" s="1">
+        <v>2696.38</v>
+      </c>
+      <c r="M107" s="1">
+        <v>2702.87</v>
+      </c>
+    </row>
+    <row r="108" spans="1:13">
       <c r="A108" s="1" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D108" s="1">
         <v>2987.82</v>
@@ -3394,10 +5008,25 @@
       <c r="H108" s="1">
         <v>3014.3</v>
       </c>
-    </row>
-    <row r="109" spans="2:8">
+      <c r="I108" s="1">
+        <v>2980.82</v>
+      </c>
+      <c r="J108" s="1">
+        <v>3266</v>
+      </c>
+      <c r="K108" s="1">
+        <v>2989.13</v>
+      </c>
+      <c r="L108" s="1">
+        <v>3002.88</v>
+      </c>
+      <c r="M108" s="1">
+        <v>2986</v>
+      </c>
+    </row>
+    <row r="109" spans="2:13">
       <c r="B109" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D109" s="1">
         <v>29.24</v>
@@ -3414,10 +5043,25 @@
       <c r="H109" s="1">
         <v>29.52</v>
       </c>
-    </row>
-    <row r="110" spans="2:8">
+      <c r="I109" s="1">
+        <v>29.45</v>
+      </c>
+      <c r="J109" s="1">
+        <v>31.31</v>
+      </c>
+      <c r="K109" s="1">
+        <v>28.77</v>
+      </c>
+      <c r="L109" s="1">
+        <v>29.88</v>
+      </c>
+      <c r="M109" s="1">
+        <v>28.77</v>
+      </c>
+    </row>
+    <row r="110" spans="2:13">
       <c r="B110" s="1" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D110" s="1">
         <v>2956.77</v>
@@ -3434,13 +5078,28 @@
       <c r="H110" s="1">
         <v>2982.99</v>
       </c>
-    </row>
-    <row r="111" spans="1:8">
+      <c r="I110" s="1">
+        <v>2949.51</v>
+      </c>
+      <c r="J110" s="1">
+        <v>3233</v>
+      </c>
+      <c r="K110" s="1">
+        <v>2957.5</v>
+      </c>
+      <c r="L110" s="1">
+        <v>2970.93</v>
+      </c>
+      <c r="M110" s="1">
+        <v>2955.36</v>
+      </c>
+    </row>
+    <row r="111" spans="1:13">
       <c r="A111" s="1" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D111" s="1">
         <v>1794.26</v>
@@ -3457,10 +5116,25 @@
       <c r="H111" s="1">
         <v>1901.87</v>
       </c>
-    </row>
-    <row r="112" spans="2:8">
+      <c r="I111" s="1">
+        <v>1786.13</v>
+      </c>
+      <c r="J111" s="1">
+        <v>1915.36</v>
+      </c>
+      <c r="K111" s="1">
+        <v>1912.96</v>
+      </c>
+      <c r="L111" s="1">
+        <v>1792.83</v>
+      </c>
+      <c r="M111" s="1">
+        <v>1784.53</v>
+      </c>
+    </row>
+    <row r="112" spans="2:13">
       <c r="B112" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D112" s="1">
         <v>16.6</v>
@@ -3477,10 +5151,25 @@
       <c r="H112" s="1">
         <v>17.11</v>
       </c>
-    </row>
-    <row r="113" spans="2:8">
+      <c r="I112" s="1">
+        <v>17.14</v>
+      </c>
+      <c r="J112" s="1">
+        <v>17.51</v>
+      </c>
+      <c r="K112" s="1">
+        <v>16.48</v>
+      </c>
+      <c r="L112" s="1">
+        <v>16.82</v>
+      </c>
+      <c r="M112" s="1">
+        <v>16.72</v>
+      </c>
+    </row>
+    <row r="113" spans="2:13">
       <c r="B113" s="1" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D113" s="1">
         <v>1778.7</v>
@@ -3497,13 +5186,28 @@
       <c r="H113" s="1">
         <v>1885.88</v>
       </c>
-    </row>
-    <row r="114" spans="1:8">
+      <c r="I113" s="1">
+        <v>1770.03</v>
+      </c>
+      <c r="J113" s="1">
+        <v>1898.9</v>
+      </c>
+      <c r="K113" s="1">
+        <v>1897.13</v>
+      </c>
+      <c r="L113" s="1">
+        <v>1776.85</v>
+      </c>
+      <c r="M113" s="1">
+        <v>1768.68</v>
+      </c>
+    </row>
+    <row r="114" spans="1:13">
       <c r="A114" s="1" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D114" s="1">
         <v>1877.42</v>
@@ -3520,10 +5224,25 @@
       <c r="H114" s="1">
         <v>1884.53</v>
       </c>
-    </row>
-    <row r="115" spans="2:8">
+      <c r="I114" s="1">
+        <v>1882.01</v>
+      </c>
+      <c r="J114" s="1">
+        <v>2021.66</v>
+      </c>
+      <c r="K114" s="1">
+        <v>1879.93</v>
+      </c>
+      <c r="L114" s="1">
+        <v>1878.33</v>
+      </c>
+      <c r="M114" s="1">
+        <v>1870.24</v>
+      </c>
+    </row>
+    <row r="115" spans="2:13">
       <c r="B115" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D115" s="1">
         <v>16.85</v>
@@ -3540,10 +5259,25 @@
       <c r="H115" s="1">
         <v>17.07</v>
       </c>
-    </row>
-    <row r="116" spans="2:8">
+      <c r="I115" s="1">
+        <v>16.83</v>
+      </c>
+      <c r="J115" s="1">
+        <v>17.65</v>
+      </c>
+      <c r="K115" s="1">
+        <v>16.61</v>
+      </c>
+      <c r="L115" s="1">
+        <v>16.35</v>
+      </c>
+      <c r="M115" s="1">
+        <v>17.15</v>
+      </c>
+    </row>
+    <row r="116" spans="2:13">
       <c r="B116" s="1" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D116" s="1">
         <v>1861.69</v>
@@ -3560,13 +5294,28 @@
       <c r="H116" s="1">
         <v>1868.57</v>
       </c>
-    </row>
-    <row r="117" spans="1:8">
+      <c r="I116" s="1">
+        <v>1866.19</v>
+      </c>
+      <c r="J116" s="1">
+        <v>2005.19</v>
+      </c>
+      <c r="K116" s="1">
+        <v>1863.88</v>
+      </c>
+      <c r="L116" s="1">
+        <v>1863.08</v>
+      </c>
+      <c r="M116" s="1">
+        <v>1853.86</v>
+      </c>
+    </row>
+    <row r="117" spans="1:13">
       <c r="A117" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D117" s="1">
         <v>1813.9</v>
@@ -3583,10 +5332,25 @@
       <c r="H117" s="1">
         <v>1812.58</v>
       </c>
-    </row>
-    <row r="118" spans="2:8">
+      <c r="I117" s="1">
+        <v>1808.63</v>
+      </c>
+      <c r="J117" s="1">
+        <v>1900.62</v>
+      </c>
+      <c r="K117" s="5">
+        <v>2860.39</v>
+      </c>
+      <c r="L117" s="1">
+        <v>1801.86</v>
+      </c>
+      <c r="M117" s="1">
+        <v>1807.34</v>
+      </c>
+    </row>
+    <row r="118" spans="2:13">
       <c r="B118" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D118" s="1">
         <v>17.11</v>
@@ -3603,10 +5367,25 @@
       <c r="H118" s="1">
         <v>17.31</v>
       </c>
-    </row>
-    <row r="119" spans="2:8">
+      <c r="I118" s="1">
+        <v>17.23</v>
+      </c>
+      <c r="J118" s="1">
+        <v>17.56</v>
+      </c>
+      <c r="K118" s="1">
+        <v>22.32</v>
+      </c>
+      <c r="L118" s="1">
+        <v>17.2</v>
+      </c>
+      <c r="M118" s="1">
+        <v>16.81</v>
+      </c>
+    </row>
+    <row r="119" spans="2:13">
       <c r="B119" s="1" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D119" s="1">
         <v>1797.86</v>
@@ -3623,13 +5402,28 @@
       <c r="H119" s="1">
         <v>1796.14</v>
       </c>
-    </row>
-    <row r="120" spans="1:8">
+      <c r="I119" s="1">
+        <v>1792.38</v>
+      </c>
+      <c r="J119" s="1">
+        <v>1884.16</v>
+      </c>
+      <c r="K119" s="1">
+        <v>2004.91</v>
+      </c>
+      <c r="L119" s="1">
+        <v>1785.54</v>
+      </c>
+      <c r="M119" s="1">
+        <v>1791.45</v>
+      </c>
+    </row>
+    <row r="120" spans="1:13">
       <c r="A120" s="1" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D120" s="1">
         <v>1888.77</v>
@@ -3646,10 +5440,25 @@
       <c r="H120" s="1">
         <v>1903.39</v>
       </c>
-    </row>
-    <row r="121" spans="2:8">
+      <c r="I120" s="1">
+        <v>1897.8</v>
+      </c>
+      <c r="J120" s="1">
+        <v>1915.7</v>
+      </c>
+      <c r="K120" s="1">
+        <v>2193.7</v>
+      </c>
+      <c r="L120" s="1">
+        <v>1887.72</v>
+      </c>
+      <c r="M120" s="1">
+        <v>1885.42</v>
+      </c>
+    </row>
+    <row r="121" spans="2:13">
       <c r="B121" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D121" s="1">
         <v>16.81</v>
@@ -3666,10 +5475,25 @@
       <c r="H121" s="1">
         <v>16.93</v>
       </c>
-    </row>
-    <row r="122" spans="2:8">
+      <c r="I121" s="1">
+        <v>16.99</v>
+      </c>
+      <c r="J121" s="1">
+        <v>17.01</v>
+      </c>
+      <c r="K121" s="1">
+        <v>18.43</v>
+      </c>
+      <c r="L121" s="1">
+        <v>16.4</v>
+      </c>
+      <c r="M121" s="1">
+        <v>17.2</v>
+      </c>
+    </row>
+    <row r="122" spans="2:13">
       <c r="B122" s="1" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D122" s="1">
         <v>1873.06</v>
@@ -3686,33 +5510,63 @@
       <c r="H122" s="1">
         <v>1887.48</v>
       </c>
-    </row>
-    <row r="123" spans="1:8">
+      <c r="I122" s="1">
+        <v>1881.74</v>
+      </c>
+      <c r="J122" s="1">
+        <v>1899.74</v>
+      </c>
+      <c r="K122" s="1">
+        <v>1932.69</v>
+      </c>
+      <c r="L122" s="1">
+        <v>1871.72</v>
+      </c>
+      <c r="M122" s="1">
+        <v>1869.29</v>
+      </c>
+    </row>
+    <row r="123" spans="1:13">
       <c r="A123" s="1" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D123" s="1">
+        <v>13</v>
+      </c>
+      <c r="D123" s="5">
         <v>4123.54</v>
       </c>
-      <c r="E123" s="1">
+      <c r="E123" s="5">
         <v>4114.03</v>
       </c>
-      <c r="F123" s="1">
+      <c r="F123" s="5">
         <v>4120.18</v>
       </c>
-      <c r="G123" s="1">
+      <c r="G123" s="5">
         <v>5124.13</v>
       </c>
-      <c r="H123" s="1">
+      <c r="H123" s="5">
         <v>4184.99</v>
       </c>
-    </row>
-    <row r="124" spans="2:8">
+      <c r="I123" s="5">
+        <v>4141.64</v>
+      </c>
+      <c r="J123" s="5">
+        <v>4413.68</v>
+      </c>
+      <c r="K123" s="5">
+        <v>4201.55</v>
+      </c>
+      <c r="L123" s="5">
+        <v>4135.61</v>
+      </c>
+      <c r="M123" s="5">
+        <v>4139.07</v>
+      </c>
+    </row>
+    <row r="124" spans="2:13">
       <c r="B124" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D124" s="1">
         <v>33.89</v>
@@ -3729,10 +5583,25 @@
       <c r="H124" s="1">
         <v>34.96</v>
       </c>
-    </row>
-    <row r="125" spans="2:8">
+      <c r="I124" s="1">
+        <v>34.43</v>
+      </c>
+      <c r="J124" s="1">
+        <v>35.73</v>
+      </c>
+      <c r="K124" s="1">
+        <v>34.41</v>
+      </c>
+      <c r="L124" s="1">
+        <v>34.51</v>
+      </c>
+      <c r="M124" s="1">
+        <v>34.28</v>
+      </c>
+    </row>
+    <row r="125" spans="2:13">
       <c r="B125" s="1" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D125" s="1">
         <v>3627.2</v>
@@ -3749,33 +5618,63 @@
       <c r="H125" s="1">
         <v>3685.15</v>
       </c>
-    </row>
-    <row r="126" spans="1:8">
+      <c r="I125" s="1">
+        <v>3644.33</v>
+      </c>
+      <c r="J125" s="1">
+        <v>3914.94</v>
+      </c>
+      <c r="K125" s="1">
+        <v>3690.94</v>
+      </c>
+      <c r="L125" s="1">
+        <v>3637.9</v>
+      </c>
+      <c r="M125" s="1">
+        <v>3642.18</v>
+      </c>
+    </row>
+    <row r="126" spans="1:13">
       <c r="A126" s="1" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D126" s="1">
+        <v>13</v>
+      </c>
+      <c r="D126" s="5">
         <v>4363.49</v>
       </c>
-      <c r="E126" s="1">
+      <c r="E126" s="5">
         <v>4365.35</v>
       </c>
-      <c r="F126" s="1">
+      <c r="F126" s="5">
         <v>4357.18</v>
       </c>
-      <c r="G126" s="1">
+      <c r="G126" s="5">
         <v>4382.03</v>
       </c>
-      <c r="H126" s="1">
+      <c r="H126" s="5">
         <v>4501.83</v>
       </c>
-    </row>
-    <row r="127" spans="2:8">
+      <c r="I126" s="5">
+        <v>4359.75</v>
+      </c>
+      <c r="J126" s="5">
+        <v>4720.85</v>
+      </c>
+      <c r="K126" s="5">
+        <v>4367.21</v>
+      </c>
+      <c r="L126" s="5">
+        <v>4358.02</v>
+      </c>
+      <c r="M126" s="5">
+        <v>4359.51</v>
+      </c>
+    </row>
+    <row r="127" spans="2:13">
       <c r="B127" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D127" s="1">
         <v>35.16</v>
@@ -3792,10 +5691,25 @@
       <c r="H127" s="1">
         <v>36.04</v>
       </c>
-    </row>
-    <row r="128" spans="2:8">
+      <c r="I127" s="1">
+        <v>33.79</v>
+      </c>
+      <c r="J127" s="1">
+        <v>36.49</v>
+      </c>
+      <c r="K127" s="1">
+        <v>33.9</v>
+      </c>
+      <c r="L127" s="1">
+        <v>35.13</v>
+      </c>
+      <c r="M127" s="1">
+        <v>34.78</v>
+      </c>
+    </row>
+    <row r="128" spans="2:13">
       <c r="B128" s="1" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D128" s="1">
         <v>3862.44</v>
@@ -3811,6 +5725,21 @@
       </c>
       <c r="H128" s="1">
         <v>4001.13</v>
+      </c>
+      <c r="I128" s="1">
+        <v>3864.04</v>
+      </c>
+      <c r="J128" s="1">
+        <v>4200.14</v>
+      </c>
+      <c r="K128" s="1">
+        <v>3871.24</v>
+      </c>
+      <c r="L128" s="1">
+        <v>3860.7</v>
+      </c>
+      <c r="M128" s="1">
+        <v>3862.88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>